<commit_message>
correlation visualization ready for lasso again
</commit_message>
<xml_diff>
--- a/curationFull.xlsx
+++ b/curationFull.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23070" windowHeight="9968" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23070" windowHeight="9968" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="twitterTextByDate" sheetId="8" r:id="rId1"/>
@@ -5770,8 +5770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6415,7 +6415,7 @@
         <v>706</v>
       </c>
       <c r="E39" s="17">
-        <v>618</v>
+        <v>718</v>
       </c>
       <c r="F39" t="s">
         <v>22</v>
@@ -7247,8 +7247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1670"/>
   <sheetViews>
-    <sheetView topLeftCell="A1647" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A1667" sqref="A1667"/>
+    <sheetView topLeftCell="A697" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A706" sqref="A706"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -26761,8 +26761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -29831,8 +29831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1726"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="A856" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R1039" sqref="R1039"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -29855,7 +29855,7 @@
     <col min="19" max="19" width="21.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="114" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:21" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A1" s="11"/>
       <c r="B1" s="11" t="s">
         <v>40</v>
@@ -52125,8 +52125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="V47" sqref="V47"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23:T49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -54005,47 +54005,47 @@
       </c>
       <c r="C38">
         <f ca="1">SUM(INDIRECT(CONCATENATE("tobi!B",twitterTextByDate!$E38)):INDIRECT(CONCATENATE("tobi!B",twitterTextByDate!$E39-1)))</f>
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="D38">
         <f ca="1">SUM(INDIRECT(CONCATENATE("tobi!C",twitterTextByDate!$E38)):INDIRECT(CONCATENATE("tobi!C",twitterTextByDate!$E39-1)))</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="E38">
         <f ca="1">SUM(INDIRECT(CONCATENATE("tobi!D",twitterTextByDate!$E38)):INDIRECT(CONCATENATE("tobi!D",twitterTextByDate!$E39-1)))</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F38">
         <f ca="1">SUM(INDIRECT(CONCATENATE("tobi!E",twitterTextByDate!$E38)):INDIRECT(CONCATENATE("tobi!E",twitterTextByDate!$E39-1)))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G38">
         <f ca="1">SUM(INDIRECT(CONCATENATE("tobi!F",twitterTextByDate!$E38)):INDIRECT(CONCATENATE("tobi!F",twitterTextByDate!$E39-1)))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H38">
         <f ca="1">SUM(INDIRECT(CONCATENATE("tobi!G",twitterTextByDate!$E38)):INDIRECT(CONCATENATE("tobi!G",twitterTextByDate!$E39-1)))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I38">
         <f ca="1">SUM(INDIRECT(CONCATENATE("tobi!H",twitterTextByDate!$E38)):INDIRECT(CONCATENATE("tobi!H",twitterTextByDate!$E39-1)))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J38">
         <f ca="1">SUM(INDIRECT(CONCATENATE("tobi!I",twitterTextByDate!$E38)):INDIRECT(CONCATENATE("tobi!I",twitterTextByDate!$E39-1)))</f>
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="K38">
         <f ca="1">SUM(INDIRECT(CONCATENATE("tobi!J",twitterTextByDate!$E38)):INDIRECT(CONCATENATE("tobi!J",twitterTextByDate!$E39-1)))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L38">
         <f ca="1">SUM(INDIRECT(CONCATENATE("tobi!K",twitterTextByDate!$E38)):INDIRECT(CONCATENATE("tobi!K",twitterTextByDate!$E39-1)))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M38">
         <f ca="1">SUM(INDIRECT(CONCATENATE("tobi!L",twitterTextByDate!$E38)):INDIRECT(CONCATENATE("tobi!L",twitterTextByDate!$E39-1)))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="N38">
         <f ca="1">SUM(INDIRECT(CONCATENATE("tobi!M",twitterTextByDate!$E38)):INDIRECT(CONCATENATE("tobi!M",twitterTextByDate!$E39-1)))</f>
@@ -54057,15 +54057,15 @@
       </c>
       <c r="P38">
         <f ca="1">SUM(INDIRECT(CONCATENATE("tobi!O",twitterTextByDate!$E38)):INDIRECT(CONCATENATE("tobi!O",twitterTextByDate!$E39-1)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q38">
         <f ca="1">SUM(INDIRECT(CONCATENATE("tobi!P",twitterTextByDate!$E38)):INDIRECT(CONCATENATE("tobi!P",twitterTextByDate!$E39-1)))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R38">
         <f ca="1">SUM(INDIRECT(CONCATENATE("tobi!Q",twitterTextByDate!$E38)):INDIRECT(CONCATENATE("tobi!Q",twitterTextByDate!$E39-1)))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S38">
         <f ca="1">SUM(INDIRECT(CONCATENATE("tobi!R",twitterTextByDate!$E38)):INDIRECT(CONCATENATE("tobi!R",twitterTextByDate!$E39-1)))</f>
@@ -54073,7 +54073,7 @@
       </c>
       <c r="T38">
         <f ca="1">SUM(INDIRECT(CONCATENATE("tobi!S",twitterTextByDate!$E38)):INDIRECT(CONCATENATE("tobi!S",twitterTextByDate!$E39-1)))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.45">
@@ -54085,47 +54085,47 @@
       </c>
       <c r="C39">
         <f ca="1">SUM(INDIRECT(CONCATENATE("tobi!B",twitterTextByDate!$E39)):INDIRECT(CONCATENATE("tobi!B",twitterTextByDate!$E40-1)))</f>
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="D39">
         <f ca="1">SUM(INDIRECT(CONCATENATE("tobi!C",twitterTextByDate!$E39)):INDIRECT(CONCATENATE("tobi!C",twitterTextByDate!$E40-1)))</f>
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="E39">
         <f ca="1">SUM(INDIRECT(CONCATENATE("tobi!D",twitterTextByDate!$E39)):INDIRECT(CONCATENATE("tobi!D",twitterTextByDate!$E40-1)))</f>
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="F39">
         <f ca="1">SUM(INDIRECT(CONCATENATE("tobi!E",twitterTextByDate!$E39)):INDIRECT(CONCATENATE("tobi!E",twitterTextByDate!$E40-1)))</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G39">
         <f ca="1">SUM(INDIRECT(CONCATENATE("tobi!F",twitterTextByDate!$E39)):INDIRECT(CONCATENATE("tobi!F",twitterTextByDate!$E40-1)))</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H39">
         <f ca="1">SUM(INDIRECT(CONCATENATE("tobi!G",twitterTextByDate!$E39)):INDIRECT(CONCATENATE("tobi!G",twitterTextByDate!$E40-1)))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I39">
         <f ca="1">SUM(INDIRECT(CONCATENATE("tobi!H",twitterTextByDate!$E39)):INDIRECT(CONCATENATE("tobi!H",twitterTextByDate!$E40-1)))</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J39">
         <f ca="1">SUM(INDIRECT(CONCATENATE("tobi!I",twitterTextByDate!$E39)):INDIRECT(CONCATENATE("tobi!I",twitterTextByDate!$E40-1)))</f>
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K39">
         <f ca="1">SUM(INDIRECT(CONCATENATE("tobi!J",twitterTextByDate!$E39)):INDIRECT(CONCATENATE("tobi!J",twitterTextByDate!$E40-1)))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L39">
         <f ca="1">SUM(INDIRECT(CONCATENATE("tobi!K",twitterTextByDate!$E39)):INDIRECT(CONCATENATE("tobi!K",twitterTextByDate!$E40-1)))</f>
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="M39">
         <f ca="1">SUM(INDIRECT(CONCATENATE("tobi!L",twitterTextByDate!$E39)):INDIRECT(CONCATENATE("tobi!L",twitterTextByDate!$E40-1)))</f>
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="N39">
         <f ca="1">SUM(INDIRECT(CONCATENATE("tobi!M",twitterTextByDate!$E39)):INDIRECT(CONCATENATE("tobi!M",twitterTextByDate!$E40-1)))</f>
@@ -54137,15 +54137,15 @@
       </c>
       <c r="P39">
         <f ca="1">SUM(INDIRECT(CONCATENATE("tobi!O",twitterTextByDate!$E39)):INDIRECT(CONCATENATE("tobi!O",twitterTextByDate!$E40-1)))</f>
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="Q39">
         <f ca="1">SUM(INDIRECT(CONCATENATE("tobi!P",twitterTextByDate!$E39)):INDIRECT(CONCATENATE("tobi!P",twitterTextByDate!$E40-1)))</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="R39">
         <f ca="1">SUM(INDIRECT(CONCATENATE("tobi!Q",twitterTextByDate!$E39)):INDIRECT(CONCATENATE("tobi!Q",twitterTextByDate!$E40-1)))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S39">
         <f ca="1">SUM(INDIRECT(CONCATENATE("tobi!R",twitterTextByDate!$E39)):INDIRECT(CONCATENATE("tobi!R",twitterTextByDate!$E40-1)))</f>
@@ -54153,7 +54153,7 @@
       </c>
       <c r="T39">
         <f ca="1">SUM(INDIRECT(CONCATENATE("tobi!S",twitterTextByDate!$E39)):INDIRECT(CONCATENATE("tobi!S",twitterTextByDate!$E40-1)))</f>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.45">
@@ -55050,8 +55050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -56930,47 +56930,47 @@
       </c>
       <c r="C38">
         <f ca="1">tobiDated!C38/totalTweetsCleaned!$C38</f>
-        <v>4.9396864287055054E-6</v>
+        <v>1.3831122000375416E-4</v>
       </c>
       <c r="D38">
         <f ca="1">tobiDated!D38/totalTweetsCleaned!$C38</f>
-        <v>0</v>
+        <v>6.9155610001877079E-5</v>
       </c>
       <c r="E38">
         <f ca="1">tobiDated!E38/totalTweetsCleaned!$C38</f>
-        <v>4.9396864287055054E-6</v>
+        <v>3.9517491429644043E-5</v>
       </c>
       <c r="F38">
         <f ca="1">tobiDated!F38/totalTweetsCleaned!$C38</f>
-        <v>0</v>
+        <v>1.9758745714822022E-5</v>
       </c>
       <c r="G38">
         <f ca="1">tobiDated!G38/totalTweetsCleaned!$C38</f>
-        <v>0</v>
+        <v>4.9396864287055054E-6</v>
       </c>
       <c r="H38">
         <f ca="1">tobiDated!H38/totalTweetsCleaned!$C38</f>
-        <v>0</v>
+        <v>4.9396864287055054E-6</v>
       </c>
       <c r="I38">
         <f ca="1">tobiDated!I38/totalTweetsCleaned!$C38</f>
-        <v>0</v>
+        <v>4.9396864287055054E-6</v>
       </c>
       <c r="J38">
         <f ca="1">tobiDated!J38/totalTweetsCleaned!$C38</f>
-        <v>9.8793728574110108E-6</v>
+        <v>6.4215923573171575E-5</v>
       </c>
       <c r="K38">
         <f ca="1">tobiDated!K38/totalTweetsCleaned!$C38</f>
-        <v>0</v>
+        <v>9.8793728574110108E-6</v>
       </c>
       <c r="L38">
         <f ca="1">tobiDated!L38/totalTweetsCleaned!$C38</f>
-        <v>0</v>
+        <v>1.4819059286116518E-5</v>
       </c>
       <c r="M38">
         <f ca="1">tobiDated!M38/totalTweetsCleaned!$C38</f>
-        <v>0</v>
+        <v>4.4457177858349554E-5</v>
       </c>
       <c r="N38">
         <f ca="1">tobiDated!N38/totalTweetsCleaned!$C38</f>
@@ -56982,15 +56982,15 @@
       </c>
       <c r="P38">
         <f ca="1">tobiDated!P38/totalTweetsCleaned!$C38</f>
-        <v>0</v>
+        <v>2.4698432143527529E-5</v>
       </c>
       <c r="Q38">
         <f ca="1">tobiDated!Q38/totalTweetsCleaned!$C38</f>
-        <v>0</v>
+        <v>1.4819059286116518E-5</v>
       </c>
       <c r="R38">
         <f ca="1">tobiDated!R38/totalTweetsCleaned!$C38</f>
-        <v>0</v>
+        <v>1.4819059286116518E-5</v>
       </c>
       <c r="S38">
         <f ca="1">tobiDated!S38/totalTweetsCleaned!$C38</f>
@@ -56998,7 +56998,7 @@
       </c>
       <c r="T38">
         <f ca="1">tobiDated!T38/totalTweetsCleaned!$C38</f>
-        <v>0</v>
+        <v>9.8793728574110108E-6</v>
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.45">
@@ -57010,47 +57010,47 @@
       </c>
       <c r="C39">
         <f ca="1">tobiDated!C39/totalTweetsCleaned!$C39</f>
-        <v>2.4957742005014236E-4</v>
+        <v>9.6427639564827737E-5</v>
       </c>
       <c r="D39">
         <f ca="1">tobiDated!D39/totalTweetsCleaned!$C39</f>
-        <v>1.5882199457736333E-4</v>
+        <v>7.9410997288681664E-5</v>
       </c>
       <c r="E39">
         <f ca="1">tobiDated!E39/totalTweetsCleaned!$C39</f>
-        <v>7.3738783196632972E-5</v>
+        <v>3.4033284552292141E-5</v>
       </c>
       <c r="F39">
         <f ca="1">tobiDated!F39/totalTweetsCleaned!$C39</f>
-        <v>3.9705498644340832E-5</v>
+        <v>1.701664227614607E-5</v>
       </c>
       <c r="G39">
         <f ca="1">tobiDated!G39/totalTweetsCleaned!$C39</f>
-        <v>2.8361070460243453E-5</v>
+        <v>2.2688856368194762E-5</v>
       </c>
       <c r="H39">
         <f ca="1">tobiDated!H39/totalTweetsCleaned!$C39</f>
-        <v>1.701664227614607E-5</v>
+        <v>1.1344428184097381E-5</v>
       </c>
       <c r="I39">
         <f ca="1">tobiDated!I39/totalTweetsCleaned!$C39</f>
-        <v>3.4033284552292141E-5</v>
+        <v>2.8361070460243453E-5</v>
       </c>
       <c r="J39">
         <f ca="1">tobiDated!J39/totalTweetsCleaned!$C39</f>
-        <v>1.8718306503760678E-4</v>
+        <v>1.2478871002507118E-4</v>
       </c>
       <c r="K39">
         <f ca="1">tobiDated!K39/totalTweetsCleaned!$C39</f>
-        <v>1.701664227614607E-5</v>
+        <v>5.6722140920486904E-6</v>
       </c>
       <c r="L39">
         <f ca="1">tobiDated!L39/totalTweetsCleaned!$C39</f>
-        <v>7.3738783196632972E-5</v>
+        <v>5.6722140920486905E-5</v>
       </c>
       <c r="M39">
         <f ca="1">tobiDated!M39/totalTweetsCleaned!$C39</f>
-        <v>1.3046092411711987E-4</v>
+        <v>7.9410997288681664E-5</v>
       </c>
       <c r="N39">
         <f ca="1">tobiDated!N39/totalTweetsCleaned!$C39</f>
@@ -57062,15 +57062,15 @@
       </c>
       <c r="P39">
         <f ca="1">tobiDated!P39/totalTweetsCleaned!$C39</f>
-        <v>1.0209985365687643E-4</v>
+        <v>7.3738783196632972E-5</v>
       </c>
       <c r="Q39">
         <f ca="1">tobiDated!Q39/totalTweetsCleaned!$C39</f>
-        <v>2.2688856368194762E-5</v>
+        <v>5.6722140920486904E-6</v>
       </c>
       <c r="R39">
         <f ca="1">tobiDated!R39/totalTweetsCleaned!$C39</f>
-        <v>1.701664227614607E-5</v>
+        <v>0</v>
       </c>
       <c r="S39">
         <f ca="1">tobiDated!S39/totalTweetsCleaned!$C39</f>
@@ -57078,7 +57078,7 @@
       </c>
       <c r="T39">
         <f ca="1">tobiDated!T39/totalTweetsCleaned!$C39</f>
-        <v>2.2688856368194762E-5</v>
+        <v>1.1344428184097381E-5</v>
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.45">

</xml_diff>